<commit_message>
added spi header to bosl GPS micro for bootloading
</commit_message>
<xml_diff>
--- a/Board-Hardware/Manufacturing/BoSL BOM Rev 0.3 GSP micro.xlsx
+++ b/Board-Hardware/Manufacturing/BoSL BOM Rev 0.3 GSP micro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\My Documents\Monash\Monash-BoSL\Board-Hardware\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DDB2B8-1D70-4244-94E0-CAE06D6FC781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE84EE3D-A869-4D0F-80D4-F87F5BA0F51F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,7 +366,7 @@
     <t>R1 / R9</t>
   </si>
   <si>
-    <t>P2 / P4 / P7</t>
+    <t>P2 / P4 / P7 / J1</t>
   </si>
 </sst>
 </file>
@@ -376,12 +376,19 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -483,36 +490,36 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -793,7 +800,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1469,10 +1476,10 @@
       </c>
     </row>
     <row r="25" spans="1:9" s="16" customFormat="1">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="24" t="s">
         <v>109</v>
       </c>
       <c r="C25" s="16" t="s">
@@ -1525,7 +1532,7 @@
       <c r="B27" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="25" t="s">
         <v>112</v>
       </c>
       <c r="D27" t="s">

</xml_diff>